<commit_message>
updated simple VSD test
</commit_message>
<xml_diff>
--- a/western_genre_breakdown.xlsx
+++ b/western_genre_breakdown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="25875" windowHeight="10545" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="25875" windowHeight="10545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2144,11 +2144,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="76268544"/>
-        <c:axId val="51596672"/>
+        <c:axId val="122798080"/>
+        <c:axId val="41030144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76268544"/>
+        <c:axId val="122798080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2157,7 +2157,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51596672"/>
+        <c:crossAx val="41030144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2165,7 +2165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51596672"/>
+        <c:axId val="41030144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2176,7 +2176,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76268544"/>
+        <c:crossAx val="122798080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4043,11 +4043,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="53067264"/>
-        <c:axId val="53192960"/>
+        <c:axId val="122800128"/>
+        <c:axId val="41066496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53067264"/>
+        <c:axId val="122800128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4056,7 +4056,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53192960"/>
+        <c:crossAx val="41066496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4064,7 +4064,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53192960"/>
+        <c:axId val="41066496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4075,7 +4075,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53067264"/>
+        <c:crossAx val="122800128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6305,11 +6305,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="103177216"/>
-        <c:axId val="128328832"/>
+        <c:axId val="122799104"/>
+        <c:axId val="41030720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103177216"/>
+        <c:axId val="122799104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6318,7 +6318,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128328832"/>
+        <c:crossAx val="41030720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6326,7 +6326,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128328832"/>
+        <c:axId val="41030720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6347,7 +6347,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103177216"/>
+        <c:crossAx val="122799104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="20"/>
@@ -7918,11 +7918,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="53064192"/>
-        <c:axId val="128329984"/>
+        <c:axId val="41324544"/>
+        <c:axId val="41068800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53064192"/>
+        <c:axId val="41324544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7931,7 +7931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128329984"/>
+        <c:crossAx val="41068800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7939,7 +7939,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128329984"/>
+        <c:axId val="41068800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7950,7 +7950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53064192"/>
+        <c:crossAx val="41324544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9520,11 +9520,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="53063680"/>
-        <c:axId val="72151552"/>
+        <c:axId val="41326080"/>
+        <c:axId val="41071680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53063680"/>
+        <c:axId val="41326080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9533,7 +9533,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72151552"/>
+        <c:crossAx val="41071680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9541,7 +9541,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72151552"/>
+        <c:axId val="41071680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9553,7 +9553,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53063680"/>
+        <c:crossAx val="41326080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100"/>
@@ -11785,11 +11785,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="128456704"/>
-        <c:axId val="72153856"/>
+        <c:axId val="41807872"/>
+        <c:axId val="110549184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="128456704"/>
+        <c:axId val="41807872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11798,7 +11798,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72153856"/>
+        <c:crossAx val="110549184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11806,7 +11806,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72153856"/>
+        <c:axId val="110549184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11817,7 +11817,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128456704"/>
+        <c:crossAx val="41807872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11963,16 +11963,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>542190</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>315057</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>175847</xdr:rowOff>
+      <xdr:rowOff>183174</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>380998</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>34436</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>117232</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>65943</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15549,7 +15549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN86"/>
   <sheetViews>
-    <sheetView topLeftCell="N29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="V65" sqref="V65"/>
     </sheetView>
   </sheetViews>
@@ -21522,7 +21522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>

</xml_diff>